<commit_message>
change 09/marzo part final
</commit_message>
<xml_diff>
--- a/files/FacturaSirius.xlsx
+++ b/files/FacturaSirius.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>Ref.</t>
   </si>
@@ -125,7 +125,13 @@
     <t>CHEQUE</t>
   </si>
   <si>
-    <t>fasdfsadf</t>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>EU</t>
   </si>
 </sst>
 </file>
@@ -478,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -609,6 +615,9 @@
       <c r="M3" s="3">
         <v>22268.07</v>
       </c>
+      <c r="P3" t="s">
+        <v>34</v>
+      </c>
       <c r="R3" s="3">
         <v>2904.53</v>
       </c>
@@ -634,6 +643,9 @@
       </c>
       <c r="M4" s="3">
         <v>38716.019999999997</v>
+      </c>
+      <c r="P4" t="s">
+        <v>35</v>
       </c>
       <c r="R4" s="3">
         <v>5049.92</v>

</xml_diff>